<commit_message>
CV consulta de totales del panel, no permitir anular dos veces el mismo valor en caja choca, reporte de caja chica con el estado
</commit_message>
<xml_diff>
--- a/FALEC-w1-core-web/WebContent/reportes/FALECPV-CajaChica.xlsx
+++ b/FALEC-w1-core-web/WebContent/reportes/FALECPV-CajaChica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/projects/gitrepositorio/FacturaElectronica-App/FALEC-w1-core-web/WebContent/reportes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BC6B32-EFFF-014A-A962-D3E7E71EB925}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45736F90-AC89-A543-8F8F-BB6EDE2FC648}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1520" yWindow="7580" windowWidth="42320" windowHeight="20280" xr2:uid="{E9788733-D204-D84A-A824-443E01B2DF94}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>ESTABLECIMEINTO :</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>REGISTRO</t>
+  </si>
+  <si>
+    <t>ESTADO</t>
   </si>
 </sst>
 </file>
@@ -145,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -157,10 +160,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -477,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F32A76B9-2613-7147-BFF0-D21843D4C7F8}">
-  <dimension ref="A2:J10"/>
+  <dimension ref="A2:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -488,27 +494,28 @@
     <col min="1" max="1" width="17.83203125" customWidth="1"/>
     <col min="2" max="3" width="17.6640625" customWidth="1"/>
     <col min="4" max="4" width="54.1640625" customWidth="1"/>
-    <col min="5" max="5" width="22.5" customWidth="1"/>
-    <col min="6" max="6" width="50.33203125" customWidth="1"/>
-    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5" customWidth="1"/>
+    <col min="5" max="6" width="22.5" customWidth="1"/>
+    <col min="7" max="7" width="50.33203125" customWidth="1"/>
+    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -516,11 +523,12 @@
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="4"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="3"/>
       <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -528,11 +536,12 @@
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="4"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="3"/>
       <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -540,11 +549,12 @@
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="4"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="3"/>
       <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -552,11 +562,12 @@
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="4"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="3"/>
       <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -564,11 +575,12 @@
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="4"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="3"/>
       <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -585,29 +597,32 @@
         <v>10</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A2:K2"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="A2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>